<commit_message>
Werkend: Storten, Afhalen, Paard selecteren bij gokken. Te doen: Paarden doen bewegen, finshen en wingeld. Zie scrum--> paardformules.txt voor (mogelijke) formules.
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\6IB\Paardrennen\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF88844C-8640-4A41-ACA8-5C76EB21E59B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F203D6-C380-4349-BFA2-334529E3ABCE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{D1B869DA-932C-4D3B-8150-40070A558BC2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>gemiddelde snelheid(paarden)</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Klaar</t>
+  </si>
+  <si>
+    <t>1e plaats weten tijdens de race</t>
+  </si>
+  <si>
+    <t>splisten-&gt;</t>
   </si>
 </sst>
 </file>
@@ -192,9 +198,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="8"/>
-      <name val="Segoe UI"/>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -217,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -225,6 +235,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -405,14 +419,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>1</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>3</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1026" name="Check Box 2" hidden="1">
@@ -421,7 +440,7 @@
                   <a14:compatExt spid="_x0000_s1026"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FA6C662-3D81-4A59-99B8-BB9C7C64541E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -461,20 +480,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>4</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1027" name="Check Box 3" hidden="1">
@@ -483,7 +507,7 @@
                   <a14:compatExt spid="_x0000_s1027"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA8DBAD-B5E5-4E57-B594-5A55EF134C70}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -523,20 +547,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>5</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1028" name="Check Box 4" hidden="1">
@@ -545,7 +574,7 @@
                   <a14:compatExt spid="_x0000_s1028"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE6A299A-0F2B-4A15-9653-5BB31413450C}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -585,20 +614,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>6</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1029" name="Check Box 5" hidden="1">
@@ -607,7 +641,7 @@
                   <a14:compatExt spid="_x0000_s1029"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BD9981E1-923C-4FC7-A562-32F73404A4E7}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -647,20 +681,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>7</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1030" name="Check Box 6" hidden="1">
@@ -669,7 +708,7 @@
                   <a14:compatExt spid="_x0000_s1030"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45BAB31C-9E7D-4713-BF44-EBD00C592E28}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000006040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -709,20 +748,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>6</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>8</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1031" name="Check Box 7" hidden="1">
@@ -731,7 +775,7 @@
                   <a14:compatExt spid="_x0000_s1031"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{013BE79D-61A0-453C-AD5C-B8C64379B225}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000007040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -771,20 +815,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>7</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1032" name="Check Box 8" hidden="1">
@@ -793,7 +842,7 @@
                   <a14:compatExt spid="_x0000_s1032"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7A425E7B-3C64-4178-9DFE-0977717ADCFD}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000008040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -833,20 +882,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>8</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1033" name="Check Box 9" hidden="1">
@@ -855,7 +909,7 @@
                   <a14:compatExt spid="_x0000_s1033"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1FF331BA-5A40-4F36-9B5C-2981D12FF832}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000009040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -895,20 +949,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>9</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>11</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1034" name="Check Box 10" hidden="1">
@@ -917,7 +976,7 @@
                   <a14:compatExt spid="_x0000_s1034"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01E5F44C-288F-4978-A32B-3DC5EE6A99E8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -957,20 +1016,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>10</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>12</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1035" name="Check Box 11" hidden="1">
@@ -979,7 +1043,7 @@
                   <a14:compatExt spid="_x0000_s1035"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7D86777C-47B9-4DBD-8BE4-D4017E23F564}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1019,20 +1083,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>11</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>13</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1036" name="Check Box 12" hidden="1">
@@ -1041,7 +1110,7 @@
                   <a14:compatExt spid="_x0000_s1036"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E017B71C-2539-461A-96F7-ADA1DA4B2B6E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1081,20 +1150,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>12</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>14</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1037" name="Check Box 13" hidden="1">
@@ -1103,7 +1177,7 @@
                   <a14:compatExt spid="_x0000_s1037"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ECBA6BC-89AC-4AF9-AD64-775EF8D0F746}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1143,20 +1217,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>13</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>15</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1038" name="Check Box 14" hidden="1">
@@ -1165,7 +1244,7 @@
                   <a14:compatExt spid="_x0000_s1038"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE53DEAE-B3B5-4B4C-A8DB-8DB0387BEE12}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1205,20 +1284,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>14</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>16</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1039" name="Check Box 15" hidden="1">
@@ -1227,7 +1311,7 @@
                   <a14:compatExt spid="_x0000_s1039"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE144E58-16B7-444E-B7F5-C523F5E69464}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00000F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1267,20 +1351,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>15</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>17</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1040" name="Check Box 16" hidden="1">
@@ -1289,7 +1378,7 @@
                   <a14:compatExt spid="_x0000_s1040"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A0AA00B-BD4D-4DCC-939A-8A515E2D7654}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000010040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1329,20 +1418,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>16</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>18</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1041" name="Check Box 17" hidden="1">
@@ -1351,7 +1445,7 @@
                   <a14:compatExt spid="_x0000_s1041"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1802CC82-761B-4109-8639-B849C2413B87}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000011040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1391,20 +1485,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>17</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>19</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1042" name="Check Box 18" hidden="1">
@@ -1413,7 +1512,7 @@
                   <a14:compatExt spid="_x0000_s1042"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{05629464-BC2B-4706-816A-7A80D3937957}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000012040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1453,20 +1552,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>18</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>20</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1043" name="Check Box 19" hidden="1">
@@ -1475,7 +1579,7 @@
                   <a14:compatExt spid="_x0000_s1043"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{948D2B1D-F1C6-4ABE-B74E-F91BFC1D242E}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000013040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1515,20 +1619,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>19</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>21</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1044" name="Check Box 20" hidden="1">
@@ -1537,7 +1646,7 @@
                   <a14:compatExt spid="_x0000_s1044"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E86AA650-96CD-4058-A0FE-E82EA4777512}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000014040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1577,20 +1686,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>20</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>22</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1045" name="Check Box 21" hidden="1">
@@ -1599,7 +1713,7 @@
                   <a14:compatExt spid="_x0000_s1045"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4137F35-02BF-4F98-A64A-3C5C9FF0E8B3}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000015040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1639,20 +1753,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>21</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>23</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1046" name="Check Box 22" hidden="1">
@@ -1661,7 +1780,7 @@
                   <a14:compatExt spid="_x0000_s1046"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83DFA969-8951-4114-8A7D-54BA5700E68D}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000016040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1701,20 +1820,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>12</xdr:col>
           <xdr:colOff>9525</xdr:colOff>
           <xdr:row>22</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="923925" cy="209550"/>
+        <xdr:to>
+          <xdr:col>13</xdr:col>
+          <xdr:colOff>419100</xdr:colOff>
+          <xdr:row>24</xdr:row>
+          <xdr:rowOff>9525</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1047" name="Check Box 23" hidden="1">
@@ -1723,7 +1847,7 @@
                   <a14:compatExt spid="_x0000_s1047"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{158997FE-D66E-4DB9-BFFA-68AB76C963A8}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000017040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1763,7 +1887,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -2082,17 +2206,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43909A-492C-4FBE-BFDC-1A3EFB983DB8}">
+  <sheetPr codeName="Blad1"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="30.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" customWidth="1"/>
@@ -2141,6 +2266,9 @@
       <c r="C2" t="s">
         <v>2</v>
       </c>
+      <c r="G2" s="4" t="s">
+        <v>46</v>
+      </c>
       <c r="H2">
         <v>1</v>
       </c>
@@ -2317,7 +2445,7 @@
         <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="J10">
         <v>2</v>
@@ -2571,9 +2699,10 @@
       <c r="C22" t="s">
         <v>41</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="3" t="s">
         <v>42</v>
       </c>
+      <c r="E22" s="3"/>
       <c r="H22">
         <v>21</v>
       </c>
@@ -2629,6 +2758,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D22:E22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>

<commit_message>
Scrum bijna vergeten aanvullen
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\6IB\Paardrennen\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA300C7-487D-47F2-868C-D904532774D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F91B11-5A5D-43F5-B41E-D79D4AF598EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{D1B869DA-932C-4D3B-8150-40070A558BC2}"/>
   </bookViews>
@@ -34,10 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="68">
-  <si>
-    <t>gemiddelde snelheid(paarden)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
   <si>
     <t>geld verloren lijsten</t>
   </si>
@@ -238,6 +235,9 @@
   </si>
   <si>
     <t>Assets paarden maken</t>
+  </si>
+  <si>
+    <t>gemiddelde snelheid paarden finalizen</t>
   </si>
 </sst>
 </file>
@@ -382,9 +382,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -395,6 +392,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -402,6 +402,20 @@
   <dxfs count="4">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -426,20 +440,6 @@
           <bgColor theme="1"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -470,7 +470,7 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A0B1FA5-3591-467C-B4F0-81D8FC84E627}" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="1" headerRowBorderDxfId="2" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A0B1FA5-3591-467C-B4F0-81D8FC84E627}" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
   <autoFilter ref="O1:T4" xr:uid="{F2716051-1728-4A60-9F8D-95D549BC807E}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{DA43F489-BC6A-4E5E-BF0A-B3DDF2173CB3}" name="ExtraNr"/>
@@ -782,12 +782,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43909A-492C-4FBE-BFDC-1A3EFB983DB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43909A-492C-4FBE-BFDC-1A3EFB983DB8}">
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,58 +820,58 @@
         <v>3</v>
       </c>
       <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>27</v>
       </c>
-      <c r="K1" t="s">
-        <v>28</v>
-      </c>
       <c r="L1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" t="s">
         <v>30</v>
       </c>
-      <c r="M1" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="R1" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>30</v>
-      </c>
-      <c r="T1" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2">
         <v>2</v>
@@ -880,16 +880,16 @@
         <v>1.5</v>
       </c>
       <c r="L2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O2">
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="Q2">
         <v>2</v>
@@ -898,27 +898,27 @@
         <v>3</v>
       </c>
       <c r="S2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J3">
         <v>0.5</v>
@@ -927,27 +927,27 @@
         <v>0.25</v>
       </c>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H4">
         <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>0.25</v>
@@ -956,14 +956,14 @@
         <v>0.25</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M4" t="s">
-        <v>65</v>
-      </c>
-      <c r="O4" s="13"/>
-      <c r="P4" s="9" t="s">
-        <v>29</v>
+        <v>64</v>
+      </c>
+      <c r="O4" s="12"/>
+      <c r="P4" s="8" t="s">
+        <v>28</v>
       </c>
       <c r="Q4">
         <f>SUM(Q2:Q3)</f>
@@ -973,24 +973,24 @@
         <f>SUM(R2:R3)</f>
         <v>3</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="12"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
       </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="H5">
         <v>4</v>
       </c>
       <c r="I5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -999,27 +999,27 @@
         <v>0.5</v>
       </c>
       <c r="L5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H6">
         <v>5</v>
       </c>
       <c r="I6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6">
         <v>0.5</v>
@@ -1028,27 +1028,27 @@
         <v>0.5</v>
       </c>
       <c r="L6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H7">
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J7">
         <v>0.5</v>
@@ -1057,62 +1057,65 @@
         <v>0.5</v>
       </c>
       <c r="L7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8">
         <v>7</v>
       </c>
       <c r="I8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J8">
         <v>2</v>
       </c>
       <c r="K8">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="L8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C9" t="s">
         <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
       </c>
       <c r="H9">
         <v>8</v>
       </c>
       <c r="I9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="L9" t="s">
+        <v>44</v>
       </c>
       <c r="M9" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1120,42 +1123,45 @@
         <v>9</v>
       </c>
       <c r="I10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="L10" t="s">
+        <v>44</v>
       </c>
       <c r="M10" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="H11">
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J11">
         <v>0.25</v>
@@ -1164,33 +1170,33 @@
         <v>0</v>
       </c>
       <c r="M11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F12" t="s">
         <v>38</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
       </c>
       <c r="H12">
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="J12">
         <v>1</v>
@@ -1199,33 +1205,33 @@
         <v>0</v>
       </c>
       <c r="M12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H13">
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J13">
         <v>2</v>
@@ -1234,33 +1240,33 @@
         <v>0</v>
       </c>
       <c r="M13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="H14">
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J14">
         <v>0.5</v>
@@ -1269,24 +1275,24 @@
         <v>0</v>
       </c>
       <c r="M14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H15">
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J15">
         <v>0.25</v>
@@ -1295,21 +1301,21 @@
         <v>0</v>
       </c>
       <c r="M15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H16">
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16">
         <v>1</v>
@@ -1318,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="M16" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="4:13" x14ac:dyDescent="0.25">
@@ -1326,7 +1332,7 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J17">
         <v>1</v>
@@ -1335,7 +1341,7 @@
         <v>0</v>
       </c>
       <c r="M17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="4:13" x14ac:dyDescent="0.25">
@@ -1343,7 +1349,7 @@
         <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0.25</v>
@@ -1352,7 +1358,7 @@
         <v>0</v>
       </c>
       <c r="M18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="4:13" x14ac:dyDescent="0.25">
@@ -1360,7 +1366,7 @@
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J19">
         <v>0.5</v>
@@ -1369,7 +1375,7 @@
         <v>0</v>
       </c>
       <c r="M19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="20" spans="4:13" x14ac:dyDescent="0.25">
@@ -1377,7 +1383,7 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J20">
         <v>3</v>
@@ -1386,7 +1392,7 @@
         <v>0</v>
       </c>
       <c r="M20" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" spans="4:13" x14ac:dyDescent="0.25">
@@ -1394,7 +1400,7 @@
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J21">
         <v>0.5</v>
@@ -1403,17 +1409,17 @@
         <v>0</v>
       </c>
       <c r="M21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="13"/>
       <c r="H22">
         <v>21</v>
       </c>
       <c r="I22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="J22">
         <v>2</v>
@@ -1422,7 +1428,7 @@
         <v>0</v>
       </c>
       <c r="M22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="4:13" x14ac:dyDescent="0.25">
@@ -1430,7 +1436,7 @@
         <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J23">
         <v>0.25</v>
@@ -1439,7 +1445,7 @@
         <v>0</v>
       </c>
       <c r="M23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="24" spans="4:13" x14ac:dyDescent="0.25">
@@ -1447,7 +1453,7 @@
         <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J24">
         <v>4</v>
@@ -1456,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="M24" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="4:13" x14ac:dyDescent="0.25">
@@ -1464,7 +1470,7 @@
         <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J25">
         <v>2</v>
@@ -1473,7 +1479,7 @@
         <v>0</v>
       </c>
       <c r="M25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="4:13" x14ac:dyDescent="0.25">
@@ -1481,7 +1487,7 @@
         <v>25</v>
       </c>
       <c r="I26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <v>1.5</v>
@@ -1490,7 +1496,7 @@
         <v>0</v>
       </c>
       <c r="M26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="4:13" x14ac:dyDescent="0.25">
@@ -1498,7 +1504,7 @@
         <v>26</v>
       </c>
       <c r="I27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J27">
         <v>6</v>
@@ -1507,13 +1513,13 @@
         <v>0</v>
       </c>
       <c r="M27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="4:13" x14ac:dyDescent="0.25">
-      <c r="H28" s="12"/>
+      <c r="H28" s="11"/>
       <c r="I28" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J28" s="4">
         <f ca="1">SUM(J2:J28)</f>
@@ -1523,18 +1529,17 @@
         <f ca="1">SUM(K2:K28)</f>
         <v>0</v>
       </c>
-      <c r="L28" s="10"/>
-      <c r="M28" s="11"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
   <tableParts count="2">
+    <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>
-    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Probleem met kringverzijzingen bij excel file opgelost
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\6IB\Paardrennen\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rll6ib\Documents\KieronParmentier\Paardrennen\PaardRennen\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9F91B11-5A5D-43F5-B41E-D79D4AF598EA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600" xr2:uid="{D1B869DA-932C-4D3B-8150-40070A558BC2}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="69">
   <si>
     <t>geld verloren lijsten</t>
   </si>
@@ -238,12 +237,15 @@
   </si>
   <si>
     <t>gemiddelde snelheid paarden finalizen</t>
+  </si>
+  <si>
+    <t>Rein</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -431,7 +433,6 @@
         <sz val="11"/>
         <color theme="0"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <fill>
@@ -455,32 +456,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A2FA3D79-897F-4774-8B80-5C5E74B66AA5}" name="Tabel1" displayName="Tabel1" ref="H1:M28" totalsRowShown="0">
-  <autoFilter ref="H1:M28" xr:uid="{C620840B-77BD-4B06-8BD7-75B852AAB660}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="H1:M28" totalsRowShown="0">
+  <autoFilter ref="H1:M28"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{A07E4312-B624-4E1E-8A5E-455BE5B3B379}" name="StoryNr"/>
-    <tableColumn id="2" xr3:uid="{F90275A9-7E2B-49ED-A45C-CE9A3019E367}" name="Beschrijving"/>
-    <tableColumn id="3" xr3:uid="{2F7DCD02-31B2-41C0-AE61-ED02925902D1}" name="Story points"/>
-    <tableColumn id="4" xr3:uid="{3A0C28B1-730D-4CE7-BDEF-D82F9911DD1F}" name="Effectieve duur"/>
-    <tableColumn id="5" xr3:uid="{E9E1C965-D916-43FD-B471-3E6825DDAFCB}" name="Wie?"/>
-    <tableColumn id="6" xr3:uid="{03018B22-2F63-42E4-A1E9-100B981F8ABD}" name="Klaar"/>
+    <tableColumn id="1" name="StoryNr"/>
+    <tableColumn id="2" name="Beschrijving"/>
+    <tableColumn id="3" name="Story points"/>
+    <tableColumn id="4" name="Effectieve duur"/>
+    <tableColumn id="5" name="Wie?"/>
+    <tableColumn id="6" name="Klaar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1A0B1FA5-3591-467C-B4F0-81D8FC84E627}" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="O1:T4" xr:uid="{F2716051-1728-4A60-9F8D-95D549BC807E}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="O1:T4"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{DA43F489-BC6A-4E5E-BF0A-B3DDF2173CB3}" name="ExtraNr"/>
-    <tableColumn id="2" xr3:uid="{F834DD31-280D-4358-9723-A52540A0F612}" name="Beschrijving"/>
-    <tableColumn id="3" xr3:uid="{1214D0BF-7C5F-4EE0-BB10-2F20B8EDCA88}" name="Story points" dataDxfId="0">
+    <tableColumn id="1" name="ExtraNr"/>
+    <tableColumn id="2" name="Beschrijving"/>
+    <tableColumn id="3" name="Story points" dataDxfId="0">
       <calculatedColumnFormula array="1">som</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{E016D177-0270-4CBE-9712-7FBF68DAC097}" name="Effectieve duur"/>
-    <tableColumn id="5" xr3:uid="{1AD80179-8A91-4473-B369-C86AFFBC758E}" name="Wie?"/>
-    <tableColumn id="6" xr3:uid="{122DA48F-F23F-4714-932E-AD1B9F3C9A54}" name="Klaar"/>
+    <tableColumn id="4" name="Effectieve duur"/>
+    <tableColumn id="5" name="Wie?"/>
+    <tableColumn id="6" name="Klaar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -782,12 +783,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D43909A-492C-4FBE-BFDC-1A3EFB983DB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1169,6 +1170,9 @@
       <c r="K11">
         <v>0</v>
       </c>
+      <c r="L11" t="s">
+        <v>68</v>
+      </c>
       <c r="M11" t="s">
         <v>65</v>
       </c>
@@ -1522,12 +1526,12 @@
         <v>28</v>
       </c>
       <c r="J28" s="4">
-        <f ca="1">SUM(J2:J28)</f>
-        <v>0</v>
+        <f>SUM(J2:J27)</f>
+        <v>34.75</v>
       </c>
       <c r="K28" s="4">
-        <f ca="1">SUM(K2:K28)</f>
-        <v>0</v>
+        <f>SUM(K2:K27)</f>
+        <v>7.5</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>

</xml_diff>

<commit_message>
winst per paard berekenen
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rll6ib\Documents\KieronParmentier\Paardrennen\PaardRennen\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gooss\Documents\Lyceum\ToegepasteInformatica\C#\Paardenrennen\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72503EAB-4983-4AA7-8463-DE71F4874C5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="28800" windowHeight="15600"/>
+    <workbookView xWindow="5760" yWindow="1716" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -245,7 +246,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -456,32 +457,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabel1" displayName="Tabel1" ref="H1:M28" totalsRowShown="0">
-  <autoFilter ref="H1:M28"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabel1" displayName="Tabel1" ref="H1:M28" totalsRowShown="0">
+  <autoFilter ref="H1:M28" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="StoryNr"/>
-    <tableColumn id="2" name="Beschrijving"/>
-    <tableColumn id="3" name="Story points"/>
-    <tableColumn id="4" name="Effectieve duur"/>
-    <tableColumn id="5" name="Wie?"/>
-    <tableColumn id="6" name="Klaar"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="StoryNr"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Beschrijving"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Story points"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Effectieve duur"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Wie?"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Klaar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="O1:T4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="O1:T4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="ExtraNr"/>
-    <tableColumn id="2" name="Beschrijving"/>
-    <tableColumn id="3" name="Story points" dataDxfId="0">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ExtraNr"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Beschrijving"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Story points" dataDxfId="0">
       <calculatedColumnFormula array="1">som</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" name="Effectieve duur"/>
-    <tableColumn id="5" name="Wie?"/>
-    <tableColumn id="6" name="Klaar"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Effectieve duur"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Wie?"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Klaar"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -783,34 +784,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H4" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="117.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="84.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="117.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -857,7 +858,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -905,7 +906,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -934,7 +935,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -977,7 +978,7 @@
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1006,7 +1007,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1035,7 +1036,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1064,7 +1065,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1093,7 +1094,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1119,7 +1120,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H10">
         <v>9</v>
       </c>
@@ -1139,7 +1140,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1168,16 +1169,16 @@
         <v>0.25</v>
       </c>
       <c r="K11">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="L11" t="s">
         <v>68</v>
       </c>
       <c r="M11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1215,7 +1216,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1250,7 +1251,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1285,7 +1286,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1311,7 +1312,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1334,7 +1335,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H17">
         <v>16</v>
       </c>
@@ -1351,7 +1352,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>17</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>18</v>
       </c>
@@ -1385,7 +1386,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>19</v>
       </c>
@@ -1402,7 +1403,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>20</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.3">
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="H22">
@@ -1438,7 +1439,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H23">
         <v>22</v>
       </c>
@@ -1455,7 +1456,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>23</v>
       </c>
@@ -1472,7 +1473,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H25">
         <v>24</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H26">
         <v>25</v>
       </c>
@@ -1506,7 +1507,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H27">
         <v>26</v>
       </c>
@@ -1523,7 +1524,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:13" x14ac:dyDescent="0.3">
       <c r="H28" s="11"/>
       <c r="I28" s="3" t="s">
         <v>28</v>
@@ -1534,7 +1535,7 @@
       </c>
       <c r="K28" s="4">
         <f>SUM(K2:K27)</f>
-        <v>8.5</v>
+        <v>8.75</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>

</xml_diff>

<commit_message>
scrum updated PS: Sepp, uw changes zijn niet compleet gepusht
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gooss\Documents\Lyceum\ToegepasteInformatica\C#\Paardenrennen\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\6IB\Paardrennen\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72503EAB-4983-4AA7-8463-DE71F4874C5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D6BC3E-038C-4A48-A1FA-F91171DB0218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="1716" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="28755" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
   <si>
     <t>geld verloren lijsten</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>Rein</t>
+  </si>
+  <si>
+    <t>Asset geselecteerd paard maken</t>
   </si>
 </sst>
 </file>
@@ -788,30 +791,30 @@
   <sheetPr codeName="Blad1"/>
   <dimension ref="A1:T28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R4" sqref="R4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="84.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="117.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.88671875" customWidth="1"/>
-    <col min="9" max="9" width="38.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.6640625" customWidth="1"/>
+    <col min="1" max="1" width="84.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="117.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" customWidth="1"/>
+    <col min="9" max="9" width="38.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.44140625" customWidth="1"/>
-    <col min="15" max="15" width="9.6640625" customWidth="1"/>
-    <col min="16" max="16" width="21.109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.6640625" customWidth="1"/>
-    <col min="18" max="18" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="13.42578125" customWidth="1"/>
+    <col min="15" max="15" width="9.7109375" customWidth="1"/>
+    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.7109375" customWidth="1"/>
+    <col min="18" max="18" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -858,7 +861,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -906,7 +909,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -934,8 +937,26 @@
       <c r="M3" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="O3">
+        <v>2</v>
+      </c>
+      <c r="P3" t="s">
+        <v>69</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" t="s">
+        <v>44</v>
+      </c>
+      <c r="T3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -969,7 +990,7 @@
       </c>
       <c r="Q4">
         <f>SUM(Q2:Q3)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="R4">
         <f>SUM(R2:R3)</f>
@@ -978,7 +999,7 @@
       <c r="S4" s="12"/>
       <c r="T4" s="12"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1007,7 +1028,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1036,7 +1057,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1065,7 +1086,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1094,7 +1115,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1120,7 +1141,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="H10">
         <v>9</v>
       </c>
@@ -1140,7 +1161,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1178,7 +1199,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1216,7 +1237,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1245,13 +1266,16 @@
         <v>2</v>
       </c>
       <c r="K13">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
       </c>
       <c r="M13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1282,11 +1306,14 @@
       <c r="K14">
         <v>0</v>
       </c>
+      <c r="L14" t="s">
+        <v>44</v>
+      </c>
       <c r="M14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1312,7 +1339,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1335,7 +1362,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H17">
         <v>16</v>
       </c>
@@ -1352,7 +1379,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H18">
         <v>17</v>
       </c>
@@ -1369,7 +1396,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H19">
         <v>18</v>
       </c>
@@ -1386,7 +1413,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H20">
         <v>19</v>
       </c>
@@ -1403,7 +1430,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H21">
         <v>20</v>
       </c>
@@ -1420,7 +1447,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="4:13" x14ac:dyDescent="0.25">
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
       <c r="H22">
@@ -1439,7 +1466,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="23" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H23">
         <v>22</v>
       </c>
@@ -1456,7 +1483,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H24">
         <v>23</v>
       </c>
@@ -1473,7 +1500,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H25">
         <v>24</v>
       </c>
@@ -1490,7 +1517,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H26">
         <v>25</v>
       </c>
@@ -1507,7 +1534,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H27">
         <v>26</v>
       </c>
@@ -1524,7 +1551,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="4:13" x14ac:dyDescent="0.3">
+    <row r="28" spans="4:13" x14ac:dyDescent="0.25">
       <c r="H28" s="11"/>
       <c r="I28" s="3" t="s">
         <v>28</v>
@@ -1535,7 +1562,7 @@
       </c>
       <c r="K28" s="4">
         <f>SUM(K2:K27)</f>
-        <v>8.75</v>
+        <v>9.75</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>

</xml_diff>

<commit_message>
lmao paard arrow lol
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\6IB\Paardrennen\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85D6BC3E-038C-4A48-A1FA-F91171DB0218}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C43505-DCB3-44C9-BFB6-D02E86224069}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="720" windowWidth="28755" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="70">
   <si>
     <t>geld verloren lijsten</t>
   </si>
@@ -378,7 +378,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -401,6 +401,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -475,8 +476,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabel3" displayName="Tabel3" ref="O1:T4" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
-  <autoFilter ref="O1:T4" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabel3" displayName="Tabel3" ref="O1:T5" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="2" tableBorderDxfId="1">
+  <autoFilter ref="O1:T5" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="ExtraNr"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Beschrijving"/>
@@ -792,7 +793,7 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -944,16 +945,16 @@
         <v>69</v>
       </c>
       <c r="Q3">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="R3">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="S3" t="s">
         <v>44</v>
       </c>
       <c r="T3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
@@ -984,20 +985,10 @@
       <c r="M4" t="s">
         <v>64</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q4">
-        <f>SUM(Q2:Q3)</f>
-        <v>3</v>
-      </c>
-      <c r="R4">
-        <f>SUM(R2:R3)</f>
-        <v>3</v>
-      </c>
-      <c r="S4" s="12"/>
-      <c r="T4" s="12"/>
+      <c r="O4" s="14"/>
+      <c r="P4" s="8"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1027,6 +1018,20 @@
       <c r="M5" t="s">
         <v>64</v>
       </c>
+      <c r="O5" s="12"/>
+      <c r="P5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q5">
+        <f>SUM($Q$2:Q4)</f>
+        <v>2.5</v>
+      </c>
+      <c r="R5">
+        <f>SUM($R$2:R4)</f>
+        <v>3.25</v>
+      </c>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -1184,16 +1189,16 @@
         <v>10</v>
       </c>
       <c r="I11" t="s">
-        <v>46</v>
+        <v>5</v>
       </c>
       <c r="J11">
-        <v>0.25</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <v>0.25</v>
+        <v>5</v>
       </c>
       <c r="L11" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="M11" t="s">
         <v>64</v>
@@ -1222,16 +1227,16 @@
         <v>11</v>
       </c>
       <c r="I12" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="J12">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K12">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="M12" t="s">
         <v>64</v>
@@ -1260,16 +1265,16 @@
         <v>12</v>
       </c>
       <c r="I13" t="s">
-        <v>31</v>
+        <v>67</v>
       </c>
       <c r="J13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K13">
         <v>1</v>
       </c>
       <c r="L13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M13" t="s">
         <v>64</v>
@@ -1298,19 +1303,19 @@
         <v>13</v>
       </c>
       <c r="I14" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
       <c r="J14">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="K14">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="M14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
@@ -1327,16 +1332,19 @@
         <v>14</v>
       </c>
       <c r="I15" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="J15">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="K15">
         <v>0</v>
       </c>
+      <c r="L15" t="s">
+        <v>44</v>
+      </c>
       <c r="M15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
@@ -1350,16 +1358,19 @@
         <v>15</v>
       </c>
       <c r="I16" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0.25</v>
       </c>
       <c r="K16">
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="L16" t="s">
+        <v>43</v>
       </c>
       <c r="M16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="4:13" x14ac:dyDescent="0.25">
@@ -1367,13 +1378,16 @@
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="J17">
         <v>1</v>
       </c>
       <c r="K17">
         <v>0</v>
+      </c>
+      <c r="L17" t="s">
+        <v>44</v>
       </c>
       <c r="M17" t="s">
         <v>65</v>
@@ -1384,10 +1398,10 @@
         <v>17</v>
       </c>
       <c r="I18" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18">
-        <v>0.25</v>
+        <v>1</v>
       </c>
       <c r="K18">
         <v>0</v>
@@ -1401,10 +1415,10 @@
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J19">
-        <v>0.5</v>
+        <v>0.25</v>
       </c>
       <c r="K19">
         <v>0</v>
@@ -1418,10 +1432,10 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J20">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="K20">
         <v>0</v>
@@ -1562,7 +1576,7 @@
       </c>
       <c r="K28" s="4">
         <f>SUM(K2:K27)</f>
-        <v>9.75</v>
+        <v>15</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>
@@ -1572,6 +1586,9 @@
     <mergeCell ref="D22:E22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="Q2:Q3 Q5" calculatedColumn="1"/>
+  </ignoredErrors>
   <tableParts count="2">
     <tablePart r:id="rId1"/>
     <tablePart r:id="rId2"/>

</xml_diff>

<commit_message>
Themas, break message,stort limit
</commit_message>
<xml_diff>
--- a/scrum/StoryOverzicht.xlsx
+++ b/scrum/StoryOverzicht.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School\6IB\Paardrennen\scrum\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\school 6ib\C#\project3\scrum\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62361F63-638C-483D-AF8F-1B9FC8380C36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF0C3339-6BD0-4BB2-B928-B2EC720200B7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="73">
   <si>
     <t>geld verloren lijsten</t>
   </si>
@@ -250,6 +250,9 @@
   </si>
   <si>
     <t xml:space="preserve">--&gt; niet aangevuld </t>
+  </si>
+  <si>
+    <t>ja</t>
   </si>
 </sst>
 </file>
@@ -412,11 +415,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -810,29 +813,29 @@
   <dimension ref="A1:T28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="84.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="117.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="95.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="117.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="71.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="95.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="38.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="1" max="1" width="84.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="117.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="95.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="117.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="71.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="95.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.88671875" customWidth="1"/>
+    <col min="9" max="9" width="38.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.42578125" customWidth="1"/>
-    <col min="15" max="15" width="9.7109375" customWidth="1"/>
-    <col min="16" max="16" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.7109375" customWidth="1"/>
-    <col min="18" max="18" width="16.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.44140625" customWidth="1"/>
+    <col min="15" max="15" width="9.6640625" customWidth="1"/>
+    <col min="16" max="16" width="30.44140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.6640625" customWidth="1"/>
+    <col min="18" max="18" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A1" s="1">
         <v>1</v>
       </c>
@@ -879,7 +882,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -927,7 +930,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>33</v>
       </c>
@@ -974,7 +977,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1007,7 +1010,7 @@
       <c r="S4" s="13"/>
       <c r="T4" s="13"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>47</v>
       </c>
@@ -1050,7 +1053,7 @@
       <c r="S5" s="12"/>
       <c r="T5" s="12"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>32</v>
       </c>
@@ -1108,7 +1111,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>56</v>
       </c>
@@ -1137,7 +1140,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>57</v>
       </c>
@@ -1163,7 +1166,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H10">
         <v>9</v>
       </c>
@@ -1183,7 +1186,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
@@ -1221,7 +1224,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>34</v>
       </c>
@@ -1259,7 +1262,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>59</v>
       </c>
@@ -1297,7 +1300,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -1335,7 +1338,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -1364,7 +1367,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -1390,7 +1393,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H17">
         <v>16</v>
       </c>
@@ -1410,7 +1413,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="18" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H18">
         <v>17</v>
       </c>
@@ -1430,88 +1433,97 @@
         <v>64</v>
       </c>
     </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H19">
         <v>18</v>
       </c>
       <c r="I19" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J19">
-        <v>0.25</v>
+        <v>1.5</v>
       </c>
       <c r="K19">
-        <v>0</v>
+        <v>1.5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>43</v>
       </c>
       <c r="M19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H20">
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="J20">
         <v>0.5</v>
       </c>
-      <c r="K20" s="16" t="s">
-        <v>70</v>
+      <c r="K20">
+        <v>0.25</v>
       </c>
       <c r="L20" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="M20" t="s">
         <v>64</v>
       </c>
-      <c r="N20" s="15" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H21">
         <v>20</v>
       </c>
       <c r="I21" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="J21">
         <v>0.5</v>
       </c>
-      <c r="K21">
-        <v>0</v>
+      <c r="K21" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="L21" t="s">
+        <v>68</v>
       </c>
       <c r="M21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D22" s="14"/>
-      <c r="E22" s="14"/>
+        <v>64</v>
+      </c>
+      <c r="N21" s="14" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.3">
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
       <c r="H22">
         <v>21</v>
       </c>
       <c r="I22" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="J22">
-        <v>2</v>
+        <v>0.25</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>0.25</v>
+      </c>
+      <c r="L22" t="s">
+        <v>43</v>
       </c>
       <c r="M22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H23">
         <v>22</v>
       </c>
       <c r="I23" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0.25</v>
@@ -1523,15 +1535,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H24">
         <v>23</v>
       </c>
       <c r="I24" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="J24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K24">
         <v>0</v>
@@ -1540,15 +1552,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H25">
         <v>24</v>
       </c>
       <c r="I25" t="s">
-        <v>6</v>
+        <v>23</v>
       </c>
       <c r="J25">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="K25">
         <v>0</v>
@@ -1557,15 +1569,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H26">
         <v>25</v>
       </c>
       <c r="I26" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J26">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="K26">
         <v>0</v>
@@ -1574,7 +1586,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H27">
         <v>26</v>
       </c>
@@ -1591,7 +1603,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="4:14" x14ac:dyDescent="0.3">
       <c r="H28" s="11"/>
       <c r="I28" s="3" t="s">
         <v>28</v>
@@ -1602,7 +1614,7 @@
       </c>
       <c r="K28" s="4">
         <f>SUM(K2:K27)</f>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L28" s="9"/>
       <c r="M28" s="10"/>

</xml_diff>